<commit_message>
Update Access Token file
</commit_message>
<xml_diff>
--- a/Access_Token.xlsx
+++ b/Access_Token.xlsx
@@ -436,12 +436,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>eyJ0eXAiOiJKV1QiLCJub25jZSI6IlVFeElrMzAtbGo1ckkwSTZBMFhnUGNVRnpjVHNXZ084cGZSc05iMDdGZGciLCJhbGciOiJSUzI1NiIsIng1dCI6IkNOdjBPSTNSd3FsSEZFVm5hb01Bc2hDSDJYRSIsImtpZCI6IkNOdjBPSTNSd3FsSEZFVm5hb01Bc2hDSDJYRSJ9.eyJhdWQiOiIwMDAwMDAwMy0wMDAwLTAwMDAtYzAwMC0wMDAwMDAwMDAwMDAiLCJpc3MiOiJodHRwczovL3N0cy53aW5kb3dzLm5ldC9mMjcyMWI1Ni0xNDkzLTQ5NzUtODY3MS01MWIzMTUxMDkzMTcvIiwiaWF0IjoxNzQ0NTUzMDM2LCJuYmYiOjE3NDQ1NTMwMzYsImV4cCI6MTc0NDU1Nzc2MCwiYWNjdCI6MCwiYWNyIjoiMSIsImFjcnMiOlsicDEiXSwiYWlvIjoiQVdRQW0vOFpBQUFBQmtyK1BFWk9maGxJY3dsN1BaVWwvZFA0dDQ1eDVyVVlWOGc5K1o2a0VMbWVKOVM1NFFzTWd5UGxzbVdnaDlXdG1GNmRtSnAwUk9qOGVvTjlZVE1vYTIxRjdFT3hyRGM2ckczbkU2ZFVTSEVzeGRWbHpqakhQWnZLYVlXRjREZlgiLCJhbXIiOlsicHdkIiwibWZhIl0sImFwcF9kaXNwbGF5bmFtZSI6InVzaW5nIGludmVudG9yeSIsImFwcGlkIjoiZDIzZmVlMjMtYjVjMy00MDU2LTkwZjMtMDIyNDRmNmYyYWI1IiwiYXBwaWRhY3IiOiIxIiwiZmFtaWx5X25hbWUiOiJUYW4iLCJnaXZlbl9uYW1lIjoiVG9uIFRoYXQiLCJpZHR5cCI6InVzZXIiLCJpcGFkZHIiOiIyNDAyOjgwMDo2Mzc4OjMwNGY6MjA1MjoyNDg6NzgwYzoyZGUxIiwibmFtZSI6IlRvbiBUaGF0IFRhbiIsIm9pZCI6IjY1OTdhMGZhLWY0ZWEtNDU1Yi05NTUxLWVjODIzMjgwMGRlYiIsIm9ucHJlbV9zaWQiOiJTLTEtNS0yMS0xNTEwNzgzNjQ3LTE2Mjk5ODU0MTktMzk1MTE2MTQwNi0xMzYzIiwicGxhdGYiOiIzIiwicHVpZCI6IjEwMDMyMDAzNzU2MDIxMzMiLCJyaCI6IjEuQVNzQVZodHk4cE1VZFVtR2NWR3pGUkNURndNQUFBQUFBQUFBd0FBQUFBQUFBQURDQUswckFBLiIsInNjcCI6IkZpbGVzLlJlYWQgRmlsZXMuUmVhZC5BbGwgU2l0ZXMuUmVhZC5BbGwgVXNlci5SZWFkIHByb2ZpbGUgb3BlbmlkIGVtYWlsIiwic2lkIjoiMDAzZGQ0MzktMGU1MC05Y2U5LWZlNDQtODk3Nzk5YTQ0OTcyIiwic2lnbmluX3N0YXRlIjpbImttc2kiXSwic3ViIjoiYk1DYkpBUlU0LUlzMWlQOGp1ZUdpMC1fSWlhR1NoaXEtZlZfdXlHdGgxTSIsInRlbmFudF9yZWdpb25fc2NvcGUiOiJBUyIsInRpZCI6ImYyNzIxYjU2LTE0OTMtNDk3NS04NjcxLTUxYjMxNTEwOTMxNyIsInVuaXF1ZV9uYW1lIjoidGFudHRAbWF5Y2hhLmNvbS52biIsInVwbiI6InRhbnR0QG1heWNoYS5jb20udm4iLCJ1dGkiOiJuRHlGLUhPbS1rS01FaGMtZG9FZUFBIiwidmVyIjoiMS4wIiwid2lkcyI6WyJiNzlmYmY0ZC0zZWY5LTQ2ODktODE0My03NmIxOTRlODU1MDkiXSwieG1zX2Z0ZCI6InNjM0lSX09mOEVIMi15OE1UQnJTbkVnd3pzSW1wUzcwa1pJU05IbTc1UVEiLCJ4bXNfaWRyZWwiOiIxIDI0IiwieG1zX3N0Ijp7InN1YiI6IkNudy1lcVRuTXNQLUhiMnNhekVuTDZ6eVhVTEN5V0hlUXJzZmlLRWhBZnMifSwieG1zX3RjZHQiOjE2OTgyMDYyMjB9.L_CKdjiM4gWoNc_te5xXQyoAltuGMhMU9OVUWpNvstHUKpmyKDPd__ZfrmgaFGXHp-G6tb4wpDUIOJxf4F6NBFt6XNMpcYvTVmVy4Uhf4zepMhRrj4uvFYgHZs7aQUoClLqcka7uKkD3UPRPA_tQ6V_uoelJTbwesm64W7O2AEkycramLUpxxA6GsfKBYuHYwOK6hAwq9_vCZAbkJpLau0yB6InrIXPrHm-UjE6EkL_CaZGILt49OEXJ_LJh4nV4hyqwbO9WVyIsX1tjo3EnPRMu0mdx3NW09O3Z6aEmvJZ-9GRrcMN7zDp-cniAywYBVoqMBY-zBhII0Q3OIJCKcg</t>
+          <t>eyJ0eXAiOiJKV1QiLCJub25jZSI6IlNTZVBrYTZnc29pbXF6V2JwdEx5Qk9lN1hHTS1LMk9ydUJUa2Y4VG8yOFUiLCJhbGciOiJSUzI1NiIsIng1dCI6IkNOdjBPSTNSd3FsSEZFVm5hb01Bc2hDSDJYRSIsImtpZCI6IkNOdjBPSTNSd3FsSEZFVm5hb01Bc2hDSDJYRSJ9.eyJhdWQiOiIwMDAwMDAwMy0wMDAwLTAwMDAtYzAwMC0wMDAwMDAwMDAwMDAiLCJpc3MiOiJodHRwczovL3N0cy53aW5kb3dzLm5ldC9mMjcyMWI1Ni0xNDkzLTQ5NzUtODY3MS01MWIzMTUxMDkzMTcvIiwiaWF0IjoxNzQ0NTU2MjgyLCJuYmYiOjE3NDQ1NTYyODIsImV4cCI6MTc0NDU2MTAwOCwiYWNjdCI6MCwiYWNyIjoiMSIsImFjcnMiOlsicDEiXSwiYWlvIjoiQVdRQW0vOFpBQUFBQ0tseWZ3alRxcmloSVBlVFhNWDBYeUF1ZXlqcmVlY0kvdWwvY1NMZWFoN25vNkN3b1lNK2NENHl0VFZVUmNHYXQ5eElVU2hna1VpRlJmdlAyWWRDbmF0MkQyU2MrbFdKUzJCUHNhN2Yybmc1M0EzbERFcGtQSlJtRXZrQy93VjAiLCJhbXIiOlsicHdkIiwibWZhIl0sImFwcF9kaXNwbGF5bmFtZSI6InVzaW5nIGludmVudG9yeSIsImFwcGlkIjoiZDIzZmVlMjMtYjVjMy00MDU2LTkwZjMtMDIyNDRmNmYyYWI1IiwiYXBwaWRhY3IiOiIxIiwiZmFtaWx5X25hbWUiOiJUYW4iLCJnaXZlbl9uYW1lIjoiVG9uIFRoYXQiLCJpZHR5cCI6InVzZXIiLCJpcGFkZHIiOiIyNDAyOjgwMDo2Mzc4OjMwNGY6MjA1MjoyNDg6NzgwYzoyZGUxIiwibmFtZSI6IlRvbiBUaGF0IFRhbiIsIm9pZCI6IjY1OTdhMGZhLWY0ZWEtNDU1Yi05NTUxLWVjODIzMjgwMGRlYiIsIm9ucHJlbV9zaWQiOiJTLTEtNS0yMS0xNTEwNzgzNjQ3LTE2Mjk5ODU0MTktMzk1MTE2MTQwNi0xMzYzIiwicGxhdGYiOiIzIiwicHVpZCI6IjEwMDMyMDAzNzU2MDIxMzMiLCJyaCI6IjEuQVNzQVZodHk4cE1VZFVtR2NWR3pGUkNURndNQUFBQUFBQUFBd0FBQUFBQUFBQURDQUswckFBLiIsInNjcCI6IkZpbGVzLlJlYWQgRmlsZXMuUmVhZC5BbGwgU2l0ZXMuUmVhZC5BbGwgVXNlci5SZWFkIHByb2ZpbGUgb3BlbmlkIGVtYWlsIiwic2lkIjoiMDAzZGQ0MzktMGU1MC05Y2U5LWZlNDQtODk3Nzk5YTQ0OTcyIiwic2lnbmluX3N0YXRlIjpbImttc2kiXSwic3ViIjoiYk1DYkpBUlU0LUlzMWlQOGp1ZUdpMC1fSWlhR1NoaXEtZlZfdXlHdGgxTSIsInRlbmFudF9yZWdpb25fc2NvcGUiOiJBUyIsInRpZCI6ImYyNzIxYjU2LTE0OTMtNDk3NS04NjcxLTUxYjMxNTEwOTMxNyIsInVuaXF1ZV9uYW1lIjoidGFudHRAbWF5Y2hhLmNvbS52biIsInVwbiI6InRhbnR0QG1heWNoYS5jb20udm4iLCJ1dGkiOiJQQnl5YV9kU2lFbUQyTGVTQmNtZEFBIiwidmVyIjoiMS4wIiwid2lkcyI6WyJiNzlmYmY0ZC0zZWY5LTQ2ODktODE0My03NmIxOTRlODU1MDkiXSwieG1zX2Z0ZCI6ImN3S0NSeHFzUXF6NUxFTldkZ0V1T2E0NGNUTVhQeS1zbTJyblJTdWQ5OWMiLCJ4bXNfaWRyZWwiOiIxIDEwIiwieG1zX3N0Ijp7InN1YiI6IkNudy1lcVRuTXNQLUhiMnNhekVuTDZ6eVhVTEN5V0hlUXJzZmlLRWhBZnMifSwieG1zX3RjZHQiOjE2OTgyMDYyMjB9.Ddo_HrM_oIJLwRn-QtJoe3H6P5MR3jSCJXE2DkdzoAk7Kn-LDL8QngrcoMcqiRsNiM6fU47bPwG9LPV6bVLAhxP8nscUO6oPSJHAX1-Fq24rSXVyEqGdcXZqhOv6mFWhjSE5fgB40JdThsutnQ8ToSTFR5oknxM_FtLCQ6xp3i99lUMTgVr9QrYr_H5NzANPUlqJ3uSq91XxTsNcUVPKfB7Go4jRKToY4UI-DMpzU8NFh6UJlYeYjJBCGJnJPHayjbP89_JHeZQx9w_khwpuVf53NdReD3LoInSYRFVXX2zmrTvfkneB1DWkXjMvUvpnSW7b5-oLO4Syqv7mcSjBRg</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1.ASsAVhty8pMUdUmGcVGzFRCTFyPuP9LDtVZAkPMCJE9vKrXCAK0rAA.AgABAwEAAABVrSpeuWamRam2jAF1XRQEAwDs_wUA9P9iYnMFcK_H3uG75CKVcbFHLQcXA5wgJrVyU5w2O5t5p5Dz5dMVmARskBEI_4JYCzFMVtDBQelpdUu752a1AcCp7TOlu7OcA99oQVNHtPKSbMDeO0DnVG0q0b8bAGSgJ7hULHarwwsiuGv82RWCZ355xp68-EHQwob48c2MJKWT2P0JNHo0bL_3ZzFtSMWa5CbL9R4pNsOnJHFnt_37pNwMRXTi-0G_MmW-9HvLCOvbUYgDf0QiUTdHo-8TznEwC3pG6cSEhIDcuNjORwjBh0qYNz7NJc9XOANsGCYmibU2lZnUoSg6ldhvKcaeaPC0aB7reFxsaYgNamNJ4zWXWyXn4A1gMrKksF1hSs83eRLTOWzj_-_PQcBbc-U9kwZTY8jCVU9Hx5KMqoJ0on5k8EoP_o3c0nZrdOnMXWZdwJSfYrpGLYCv4gfU8Z32JrZXSWMl1Rp4GgVyJYx1x_-2j9xB1yufjboa-1pwphdMuVF8JiAmbOYZKxvq6fGZ0a2KEoFwJ3ALn8CxSKIFZTxgihXVAG__YeiQAwMGweO5spQTw8e69obgg90MIcs1-yDkj3t40LWgRMBKXEbII-mE76-GkcICZ9kEK6zVzTmdXB-cP6rl3wMODTQnpbv4ipgdaG37ulAvM8Iu5R0YXjtmT57C2LD3Tlh5RJC0DDLISSvF5NoGlz5ZoMCmnv3LGP5fYARo6rCfNJpxCRCRaIBflFOQ6JjeuDApqZIsuBVxYoY0IsO8FE_Dmp0Rf0yokNBoimQ6AoLOhUDM0b2EmPq112Q6F_1Kf2_EERYSSTD-HnUOvhLmBua2EAJejZ02nmgGqK9r2j3LrpmLiwqp071xZuYReAlIFJU</t>
+          <t>1.ASsAVhty8pMUdUmGcVGzFRCTFyPuP9LDtVZAkPMCJE9vKrXCAK0rAA.AgABAwEAAABVrSpeuWamRam2jAF1XRQEAwDs_wUA9P-0PXPg6rfuLnC8XmEg4lNLPyyB_9uvAw9k9xD7ZvgIz0m8ox4f3v5jxuOOqenz6xAZYrDz-GnyAK0tWk8uK8volxw0fBTg-jqncsUtBqPjZo8JgDTp5j5DFvAWeEMOQrjLmLk4nbtoFQ02giX11B4l23KFNxSThBrhb5g9J3MD_vEpcY3txL-byTZBYnSYepswBfl9nBqdQuNZyakhr-vxBPmxMmW7cUNJxxaBKnywKPseb5-nu8s16DaIb3dpY7B-h6jIOyu6WsHOCDdXo6ln2x0DEU7sXKTPuz6EFdcXFiYvn5JRLlQAip1eZSEo9X9ZmAaSeC12SArYbYrF_9qG3EX6rx_MrcylRqR4eL2OUQWxW_2tA3aPZ-Z_OTsKQKXZzMHzm80SsQ6gk6WrfCu5Zb-nsPxXLZUtzLHlLy4C658X9IhjG6Y0CGaArQzvF4Gl_ZZTn7D6bMYJ3df7s3gXPqtz2bhJRbpS3BZHaLBzm2fHB-FvdBCU09BT350kllvMMopLlX0OZIGo-227LWwx5_WYJUiIUDsUmRmegBwHaocafrCl8zKyOcE6xu-CYuEnk_Ir-KylkFKwv6V9tffvTLRxjdP4I78OeoIutRCf0AdOj7pC0O24umZoHv6JyTLZuTEqMkEwu-r4rVFw0slaXV-KdJ-wFS37kpjRTgOG8hJj6l9x-8IRfolUzMBnVkXZ5M03M-BQ7FxslFAxYSKQnhkhZWNO3VrV3b20WHWK_atq1XayErGrrJ_43qjQF-AL2mwgLbxcP3JfuynYqkzCBEiX3qaXgxBoOggL6buil5QiK6Gp5_C5AkakGxxLGPLrxd1roPWdx76TBtJioDQOwoNAJz4</t>
         </is>
       </c>
     </row>

</xml_diff>